<commit_message>
Usage SQL and bug servidor
</commit_message>
<xml_diff>
--- a/resources/usage_fan_in_file.xlsx
+++ b/resources/usage_fan_in_file.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Total-DB</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total-Project</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Rate</t>
         </is>
       </c>
     </row>
@@ -473,10 +483,16 @@
         <v>62</v>
       </c>
       <c r="D2" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E2" t="n">
-        <v>276</v>
+        <v>339</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4890</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6.932515337423313</v>
       </c>
     </row>
     <row r="3">
@@ -495,7 +511,13 @@
         <v>282</v>
       </c>
       <c r="E3" t="n">
-        <v>400</v>
+        <v>425</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2538</v>
+      </c>
+      <c r="G3" t="n">
+        <v>16.74546887312845</v>
       </c>
     </row>
     <row r="4">
@@ -511,10 +533,16 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" t="n">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="F4" t="n">
+        <v>8149</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.4295005522149957</v>
       </c>
     </row>
     <row r="5">
@@ -533,7 +561,13 @@
         <v>6</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2587</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.4252029377657518</v>
       </c>
     </row>
     <row r="6">
@@ -552,64 +586,13 @@
         <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>docker-java</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>languagetool</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>3</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-      <c r="D8" t="n">
-        <v>17</v>
-      </c>
-      <c r="E8" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>ebean</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3398</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.4120070629782225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New file that count the number of code and test
</commit_message>
<xml_diff>
--- a/resources/usage_fan_in_file.xlsx
+++ b/resources/usage_fan_in_file.xlsx
@@ -477,22 +477,22 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
         <v>62</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E2" t="n">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="F2" t="n">
         <v>4899</v>
       </c>
       <c r="G2" t="n">
-        <v>1.285976729944887</v>
+        <v>1.816697285160237</v>
       </c>
     </row>
     <row r="3">
@@ -502,22 +502,22 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="C3" t="n">
         <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E3" t="n">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="F3" t="n">
         <v>2538</v>
       </c>
       <c r="G3" t="n">
-        <v>1.024428684003152</v>
+        <v>4.964539007092199</v>
       </c>
     </row>
     <row r="4">
@@ -527,13 +527,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>4</v>
@@ -558,16 +558,16 @@
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="n">
         <v>2587</v>
       </c>
       <c r="G5" t="n">
-        <v>0.154619250096637</v>
+        <v>0.1159644375724778</v>
       </c>
     </row>
     <row r="6">
@@ -577,22 +577,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>202</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>335</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>538</v>
       </c>
       <c r="F6" t="n">
         <v>14079</v>
       </c>
       <c r="G6" t="n">
-        <v>0.01420555437175936</v>
+        <v>3.821294126003268</v>
       </c>
     </row>
     <row r="7">
@@ -602,22 +602,22 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F7" t="n">
         <v>3398</v>
       </c>
       <c r="G7" t="n">
-        <v>0.05885815185403178</v>
+        <v>0.1177163037080636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>